<commit_message>
Copy-edited manuscript with minor data and script adjustments
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/Metal_measures.xlsx
+++ b/analysis/data/raw_data/Metal_measures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mikkel\Saxo2020\courses\R for Archaology (DIALPAST)\PrestigeObjects\prestigeObjects\analysis\data\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mikkel\Saxo2020\papers and conferences\_papers\QuantWealth\analysis\data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="278">
   <si>
     <t>GraveID</t>
   </si>
@@ -335,9 +335,6 @@
   </si>
   <si>
     <t>2-2,5</t>
-  </si>
-  <si>
-    <t>3,9 (silver hair-ring)</t>
   </si>
   <si>
     <t>5 (measured from drawing (2:3 ratio)</t>
@@ -830,12 +827,6 @@
     <t>height/width (ie. diameters) mean (rings)</t>
   </si>
   <si>
-    <t>circumferencemm3  (calculated from mean diameter)</t>
-  </si>
-  <si>
-    <t>volume_mm3</t>
-  </si>
-  <si>
     <t>height 154.5</t>
   </si>
   <si>
@@ -858,13 +849,31 @@
   </si>
   <si>
     <t>object_description</t>
+  </si>
+  <si>
+    <t>circumference mm3  (calculated from mean diameter)</t>
+  </si>
+  <si>
+    <t>volume_mm3_numeric</t>
+  </si>
+  <si>
+    <t>weight_pure_g</t>
+  </si>
+  <si>
+    <t>dim.ratio based on length of this awl (23 mm) divided by length of reference awl (47 mm)</t>
+  </si>
+  <si>
+    <t>dim.ratio based on length of this awl (62 mm) divided by length of reference awl (47 mm)</t>
+  </si>
+  <si>
+    <t>3,9 (silver hair-ring, solid wire-based, mean diam. 21,1 mm)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -879,12 +888,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -942,7 +945,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -980,12 +983,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1011,9 +1076,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1054,18 +1116,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1092,16 +1142,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1385,8 +1453,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1400,8 +1470,8 @@
     <col min="13" max="13" width="13.54296875" customWidth="1"/>
     <col min="16" max="16" width="13.54296875" customWidth="1"/>
     <col min="18" max="19" width="10.36328125" customWidth="1"/>
-    <col min="20" max="20" width="14.7265625" style="33" customWidth="1"/>
-    <col min="21" max="21" width="13.90625" style="33" customWidth="1"/>
+    <col min="20" max="20" width="14.7265625" style="32" customWidth="1"/>
+    <col min="21" max="21" width="13.90625" style="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
@@ -1409,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1427,10 +1497,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
@@ -1442,13 +1512,13 @@
         <v>22</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>97</v>
@@ -1457,45 +1527,45 @@
         <v>90</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="T1" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="U1" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="T1" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="U1" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="V1" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="W1" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="V1" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="W1" s="35" t="s">
-        <v>195</v>
-      </c>
-      <c r="X1" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y1" s="35" t="s">
+      <c r="X1" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y1" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z1" s="34" t="s">
         <v>201</v>
       </c>
-      <c r="Z1" s="35" t="s">
-        <v>202</v>
-      </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B2" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" t="s">
         <v>212</v>
-      </c>
-      <c r="D2" t="s">
-        <v>213</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -1522,10 +1592,10 @@
         <v>936</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q2" s="6">
         <v>7.07</v>
@@ -1536,45 +1606,45 @@
       <c r="S2" s="6">
         <v>7.07</v>
       </c>
-      <c r="T2" s="29"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="35"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="34"/>
     </row>
     <row r="3" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="43" t="s">
-        <v>211</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>217</v>
+      <c r="A3" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>216</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="E3" s="45">
-        <v>1</v>
-      </c>
-      <c r="F3" s="45">
-        <v>1</v>
-      </c>
-      <c r="G3" s="45">
+        <v>213</v>
+      </c>
+      <c r="E3" s="40">
+        <v>1</v>
+      </c>
+      <c r="F3" s="40">
+        <v>1</v>
+      </c>
+      <c r="G3" s="40">
         <v>88</v>
       </c>
-      <c r="H3" s="45">
+      <c r="H3" s="40">
         <v>7</v>
       </c>
-      <c r="I3" s="45">
+      <c r="I3" s="40">
         <v>3</v>
       </c>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
       <c r="M3" s="11">
         <v>3.21</v>
       </c>
@@ -1582,7 +1652,7 @@
         <v>1848</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P3" s="13" t="s">
         <v>99</v>
@@ -1596,13 +1666,13 @@
       <c r="S3" s="11">
         <v>10.3</v>
       </c>
-      <c r="T3" s="46"/>
-      <c r="U3" s="47"/>
-      <c r="V3" s="48"/>
-      <c r="W3" s="48"/>
-      <c r="X3" s="48"/>
-      <c r="Y3" s="48"/>
-      <c r="Z3" s="48"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="42"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
+      <c r="X3" s="43"/>
+      <c r="Y3" s="43"/>
+      <c r="Z3" s="43"/>
     </row>
     <row r="4" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
@@ -1638,12 +1708,12 @@
       <c r="S4" s="15">
         <v>6.19</v>
       </c>
-      <c r="T4" s="34"/>
-      <c r="V4" s="34">
+      <c r="T4" s="33"/>
+      <c r="V4" s="33">
         <v>49.52</v>
       </c>
       <c r="W4" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="X4" s="15">
         <v>63.52</v>
@@ -1683,10 +1753,10 @@
       <c r="S5" s="13">
         <v>3.31</v>
       </c>
-      <c r="T5" s="37">
+      <c r="T5" s="56">
         <v>7.11</v>
       </c>
-      <c r="U5" s="37">
+      <c r="U5" s="56">
         <f>T5/200</f>
         <v>3.5549999999999998E-2</v>
       </c>
@@ -1708,10 +1778,10 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K6" s="16">
         <v>3</v>
@@ -1724,10 +1794,10 @@
         <v>1016.8</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q6" s="16">
         <v>3.8</v>
@@ -1738,8 +1808,8 @@
       <c r="S6" s="16">
         <v>3.8</v>
       </c>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
+      <c r="T6" s="56"/>
+      <c r="U6" s="56"/>
     </row>
     <row r="7" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
@@ -1767,7 +1837,7 @@
         <v>0.85</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>103</v>
+        <v>277</v>
       </c>
       <c r="Q7" s="8">
         <v>3.32</v>
@@ -1778,10 +1848,10 @@
       <c r="S7" s="8">
         <v>2.82</v>
       </c>
-      <c r="T7" s="23">
+      <c r="T7" s="22">
         <v>2.82</v>
       </c>
-      <c r="U7" s="24">
+      <c r="U7" s="23">
         <f>T7/200</f>
         <v>1.41E-2</v>
       </c>
@@ -1815,7 +1885,7 @@
         <v>0.92</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>103</v>
+        <v>277</v>
       </c>
       <c r="Q8" s="8">
         <v>3.6</v>
@@ -1826,10 +1896,10 @@
       <c r="S8" s="8">
         <v>3.05</v>
       </c>
-      <c r="T8" s="36">
+      <c r="T8" s="55">
         <v>108.12</v>
       </c>
-      <c r="U8" s="36">
+      <c r="U8" s="55">
         <f>T8/200</f>
         <v>0.54059999999999997</v>
       </c>
@@ -1866,10 +1936,10 @@
         <v>10997.36</v>
       </c>
       <c r="O9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q9">
         <v>37.270000000000003</v>
@@ -1880,30 +1950,30 @@
       <c r="S9">
         <v>37.270000000000003</v>
       </c>
-      <c r="T9" s="36"/>
-      <c r="U9" s="36"/>
+      <c r="T9" s="55"/>
+      <c r="U9" s="55"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E10" s="39">
+        <v>128</v>
+      </c>
+      <c r="E10" s="58">
         <v>1</v>
       </c>
       <c r="F10">
         <v>60</v>
       </c>
       <c r="I10" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -1916,36 +1986,36 @@
         <v>105</v>
       </c>
       <c r="P10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="S10">
         <v>23.4</v>
       </c>
-      <c r="T10" s="36"/>
-      <c r="U10" s="36"/>
+      <c r="T10" s="55"/>
+      <c r="U10" s="55"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="58"/>
       <c r="F11">
         <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -1958,16 +2028,16 @@
         <v>496</v>
       </c>
       <c r="P11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="S11">
         <v>44.4</v>
       </c>
-      <c r="T11" s="36"/>
-      <c r="U11" s="36"/>
+      <c r="T11" s="55"/>
+      <c r="U11" s="55"/>
     </row>
     <row r="12" spans="1:26" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
@@ -1977,7 +2047,7 @@
         <v>41</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E12" s="14">
         <v>1</v>
@@ -1995,19 +2065,19 @@
         <v>1.5</v>
       </c>
       <c r="M12" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N12" s="14">
         <v>1969</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q12" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="R12" s="14" t="s">
         <v>96</v>
@@ -2015,10 +2085,10 @@
       <c r="S12" s="14">
         <v>14.58</v>
       </c>
-      <c r="T12" s="30">
+      <c r="T12" s="29">
         <v>14.58</v>
       </c>
-      <c r="U12" s="26">
+      <c r="U12" s="25">
         <f>T12/200</f>
         <v>7.2900000000000006E-2</v>
       </c>
@@ -2049,7 +2119,7 @@
         <v>1.33</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>103</v>
+        <v>277</v>
       </c>
       <c r="Q13" s="8">
         <v>5.19</v>
@@ -2060,27 +2130,27 @@
       <c r="S13" s="8">
         <v>5.19</v>
       </c>
-      <c r="T13" s="23">
+      <c r="T13" s="22">
         <v>5.19</v>
       </c>
-      <c r="U13" s="24">
+      <c r="U13" s="23">
         <f>T13/200</f>
         <v>2.5950000000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:26" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="45" t="s">
+        <v>228</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="B14" s="53" t="s">
-        <v>235</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>230</v>
-      </c>
       <c r="E14" s="8">
         <v>1</v>
       </c>
@@ -2088,13 +2158,13 @@
         <v>1</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H14" s="8">
         <v>14.5</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M14" s="8">
         <v>0.04</v>
@@ -2103,10 +2173,10 @@
         <v>855.5</v>
       </c>
       <c r="O14" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="P14" s="14" t="s">
         <v>252</v>
-      </c>
-      <c r="P14" s="14" t="s">
-        <v>253</v>
       </c>
       <c r="Q14" s="8">
         <v>6.48</v>
@@ -2114,21 +2184,21 @@
       <c r="S14" s="8">
         <v>6.48</v>
       </c>
-      <c r="T14" s="49"/>
-      <c r="U14" s="25"/>
+      <c r="T14" s="44"/>
+      <c r="U14" s="24"/>
     </row>
     <row r="15" spans="1:26" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="51" t="s">
-        <v>229</v>
+      <c r="A15" s="46" t="s">
+        <v>228</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E15" s="13">
         <v>1</v>
@@ -2137,13 +2207,13 @@
         <v>1</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M15" s="13">
         <v>0.628</v>
@@ -2152,7 +2222,7 @@
         <v>361.8</v>
       </c>
       <c r="O15" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P15" s="13">
         <v>2.59</v>
@@ -2163,21 +2233,21 @@
       <c r="S15" s="13">
         <v>1.63</v>
       </c>
-      <c r="T15" s="52"/>
-      <c r="U15" s="27"/>
+      <c r="T15" s="47"/>
+      <c r="U15" s="26"/>
     </row>
     <row r="16" spans="1:26" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="50" t="s">
-        <v>229</v>
+      <c r="A16" s="45" t="s">
+        <v>228</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E16" s="8">
         <v>1</v>
@@ -2201,7 +2271,7 @@
         <v>12.56</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Q16" s="8">
         <v>0.56999999999999995</v>
@@ -2212,12 +2282,12 @@
       <c r="S16" s="8">
         <v>0.56999999999999995</v>
       </c>
-      <c r="T16" s="49"/>
-      <c r="U16" s="25"/>
+      <c r="T16" s="44"/>
+      <c r="U16" s="24"/>
     </row>
     <row r="17" spans="1:21" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="50" t="s">
-        <v>229</v>
+      <c r="A17" s="45" t="s">
+        <v>228</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>93</v>
@@ -2226,7 +2296,7 @@
         <v>44</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E17" s="8">
         <v>1</v>
@@ -2235,28 +2305,28 @@
         <v>2</v>
       </c>
       <c r="G17" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="M17" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="H17" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="M17" s="8" t="s">
-        <v>246</v>
-      </c>
       <c r="Q17" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="R17" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="S17" s="8">
         <v>0.1</v>
       </c>
-      <c r="T17" s="49"/>
-      <c r="U17" s="25"/>
+      <c r="T17" s="44"/>
+      <c r="U17" s="24"/>
     </row>
     <row r="18" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
@@ -2289,10 +2359,10 @@
       <c r="S18" s="8">
         <v>3.67</v>
       </c>
-      <c r="T18" s="22">
+      <c r="T18" s="21">
         <v>3.67</v>
       </c>
-      <c r="U18" s="24">
+      <c r="U18" s="23">
         <f>T18/200</f>
         <v>1.8349999999999998E-2</v>
       </c>
@@ -2328,10 +2398,10 @@
       <c r="S19" s="8">
         <v>3.67</v>
       </c>
-      <c r="T19" s="22">
+      <c r="T19" s="21">
         <v>3.67</v>
       </c>
-      <c r="U19" s="24">
+      <c r="U19" s="23">
         <f>T19/200</f>
         <v>1.8349999999999998E-2</v>
       </c>
@@ -2353,16 +2423,16 @@
         <v>4</v>
       </c>
       <c r="G20" t="s">
+        <v>111</v>
+      </c>
+      <c r="I20" t="s">
+        <v>110</v>
+      </c>
+      <c r="J20" t="s">
+        <v>107</v>
+      </c>
+      <c r="K20" t="s">
         <v>112</v>
-      </c>
-      <c r="I20" t="s">
-        <v>111</v>
-      </c>
-      <c r="J20" t="s">
-        <v>108</v>
-      </c>
-      <c r="K20" t="s">
-        <v>113</v>
       </c>
       <c r="M20">
         <v>1.39</v>
@@ -2371,10 +2441,10 @@
         <v>383</v>
       </c>
       <c r="O20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q20">
         <v>1.43</v>
@@ -2385,10 +2455,10 @@
       <c r="S20">
         <v>1.43</v>
       </c>
-      <c r="T20" s="38">
+      <c r="T20" s="57">
         <v>4.91</v>
       </c>
-      <c r="U20" s="38">
+      <c r="U20" s="57">
         <f>T20/200</f>
         <v>2.4550000000000002E-2</v>
       </c>
@@ -2422,7 +2492,7 @@
         <v>1.05</v>
       </c>
       <c r="P21" s="8" t="s">
-        <v>103</v>
+        <v>277</v>
       </c>
       <c r="Q21" s="8">
         <v>4.0999999999999996</v>
@@ -2433,8 +2503,8 @@
       <c r="S21" s="8">
         <v>3.48</v>
       </c>
-      <c r="T21" s="38"/>
-      <c r="U21" s="38"/>
+      <c r="T21" s="57"/>
+      <c r="U21" s="57"/>
     </row>
     <row r="22" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
@@ -2458,6 +2528,9 @@
       <c r="M22" s="13">
         <v>1.32</v>
       </c>
+      <c r="O22" s="13" t="s">
+        <v>276</v>
+      </c>
       <c r="P22" s="13" t="s">
         <v>99</v>
       </c>
@@ -2470,10 +2543,10 @@
       <c r="S22" s="13">
         <v>3.42</v>
       </c>
-      <c r="T22" s="31">
+      <c r="T22" s="30">
         <v>3.42</v>
       </c>
-      <c r="U22" s="27">
+      <c r="U22" s="26">
         <f>T22/200</f>
         <v>1.7100000000000001E-2</v>
       </c>
@@ -2498,7 +2571,7 @@
         <v>40</v>
       </c>
       <c r="H23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M23">
         <v>0.73</v>
@@ -2507,7 +2580,7 @@
         <v>200</v>
       </c>
       <c r="P23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q23">
         <v>0.75</v>
@@ -2518,10 +2591,10 @@
       <c r="S23">
         <v>0.75</v>
       </c>
-      <c r="T23" s="38">
+      <c r="T23" s="57">
         <v>2.02</v>
       </c>
-      <c r="U23" s="38">
+      <c r="U23" s="57">
         <f>T23/200</f>
         <v>1.01E-2</v>
       </c>
@@ -2551,6 +2624,9 @@
       <c r="M24" s="13">
         <v>0.49</v>
       </c>
+      <c r="O24" s="13" t="s">
+        <v>275</v>
+      </c>
       <c r="P24" s="13" t="s">
         <v>99</v>
       </c>
@@ -2563,16 +2639,16 @@
       <c r="S24" s="13">
         <v>1.27</v>
       </c>
-      <c r="T24" s="38"/>
-      <c r="U24" s="38"/>
+      <c r="T24" s="57"/>
+      <c r="U24" s="57"/>
     </row>
     <row r="25" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>135</v>
-      </c>
       <c r="E25" s="8">
         <v>1</v>
       </c>
@@ -2580,10 +2656,10 @@
         <v>1</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M25" s="8">
         <v>0.76</v>
@@ -2592,10 +2668,10 @@
         <v>120.89</v>
       </c>
       <c r="O25" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P25" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q25" s="8">
         <v>1.33</v>
@@ -2606,35 +2682,35 @@
       <c r="S25" s="8">
         <v>1.33</v>
       </c>
-      <c r="T25" s="23">
+      <c r="T25" s="22">
         <v>1.33</v>
       </c>
-      <c r="U25" s="24">
+      <c r="U25" s="23">
         <f>T25/200</f>
         <v>6.6500000000000005E-3</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" t="s">
+        <v>159</v>
+      </c>
+      <c r="D26" t="s">
         <v>154</v>
       </c>
-      <c r="C26" t="s">
-        <v>160</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="J26" t="s">
         <v>155</v>
       </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>156</v>
-      </c>
-      <c r="K26" t="s">
-        <v>157</v>
       </c>
       <c r="M26">
         <v>0.62</v>
@@ -2643,10 +2719,10 @@
         <v>1190.6199999999999</v>
       </c>
       <c r="O26" t="s">
+        <v>157</v>
+      </c>
+      <c r="P26" s="6" t="s">
         <v>158</v>
-      </c>
-      <c r="P26" s="6" t="s">
-        <v>159</v>
       </c>
       <c r="Q26">
         <v>13.11</v>
@@ -2657,35 +2733,35 @@
       <c r="S26">
         <v>13.11</v>
       </c>
-      <c r="T26" s="38">
+      <c r="T26" s="57">
         <v>25.87</v>
       </c>
-      <c r="U26" s="38">
+      <c r="U26" s="57">
         <f>T26/200</f>
         <v>0.12934999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C27" t="s">
+        <v>161</v>
+      </c>
+      <c r="D27" t="s">
+        <v>160</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="J27" t="s">
+        <v>163</v>
+      </c>
+      <c r="K27" t="s">
         <v>162</v>
-      </c>
-      <c r="D27" t="s">
-        <v>161</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="J27" t="s">
-        <v>164</v>
-      </c>
-      <c r="K27" t="s">
-        <v>163</v>
       </c>
       <c r="M27">
         <v>7.29</v>
@@ -2694,10 +2770,10 @@
         <v>1156.73</v>
       </c>
       <c r="O27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q27">
         <v>12.76</v>
@@ -2708,27 +2784,27 @@
       <c r="S27">
         <v>12.76</v>
       </c>
-      <c r="T27" s="38"/>
-      <c r="U27" s="38"/>
+      <c r="T27" s="57"/>
+      <c r="U27" s="57"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>165</v>
+      </c>
+      <c r="C28" t="s">
+        <v>167</v>
+      </c>
+      <c r="D28" t="s">
         <v>166</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
         <v>168</v>
-      </c>
-      <c r="D28" t="s">
-        <v>167</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="J28" t="s">
-        <v>169</v>
       </c>
       <c r="K28">
         <v>1.5</v>
@@ -2740,10 +2816,10 @@
         <v>401.05</v>
       </c>
       <c r="O28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P28" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q28">
         <v>4.43</v>
@@ -2754,23 +2830,23 @@
       <c r="S28">
         <v>4.43</v>
       </c>
-      <c r="T28" s="32">
+      <c r="T28" s="31">
         <v>4.43</v>
       </c>
-      <c r="U28" s="28">
+      <c r="U28" s="27">
         <f>T28/200</f>
         <v>2.215E-2</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>169</v>
+      </c>
+      <c r="C29" t="s">
         <v>170</v>
       </c>
-      <c r="C29" t="s">
-        <v>171</v>
-      </c>
       <c r="D29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -2779,7 +2855,7 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M29">
         <v>3.42</v>
@@ -2788,10 +2864,10 @@
         <v>942.63</v>
       </c>
       <c r="O29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q29">
         <v>3.52</v>
@@ -2802,35 +2878,35 @@
       <c r="S29">
         <v>3.52</v>
       </c>
-      <c r="T29" s="32">
+      <c r="T29" s="31">
         <v>3.52</v>
       </c>
-      <c r="U29" s="28">
+      <c r="U29" s="27">
         <f>T29/200</f>
         <v>1.7600000000000001E-2</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>179</v>
+      </c>
+      <c r="C30" t="s">
         <v>180</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
+        <v>182</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="J30" t="s">
+        <v>183</v>
+      </c>
+      <c r="K30" t="s">
         <v>181</v>
-      </c>
-      <c r="D30" t="s">
-        <v>183</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="J30" t="s">
-        <v>184</v>
-      </c>
-      <c r="K30" t="s">
-        <v>182</v>
       </c>
       <c r="M30">
         <v>3.38</v>
@@ -2839,7 +2915,7 @@
         <v>536.54999999999995</v>
       </c>
       <c r="P30" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q30">
         <v>5.92</v>
@@ -2850,32 +2926,32 @@
       <c r="S30">
         <v>5.92</v>
       </c>
-      <c r="T30" s="32">
+      <c r="T30" s="31">
         <v>5.92</v>
       </c>
-      <c r="U30" s="28">
+      <c r="U30" s="27">
         <f>T30/200</f>
         <v>2.9600000000000001E-2</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>184</v>
+      </c>
+      <c r="C31" t="s">
+        <v>186</v>
+      </c>
+      <c r="D31" t="s">
         <v>185</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="J31" t="s">
         <v>187</v>
-      </c>
-      <c r="D31" t="s">
-        <v>186</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="J31" t="s">
-        <v>188</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -2887,10 +2963,10 @@
         <v>224.52</v>
       </c>
       <c r="O31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q31">
         <v>2.48</v>
@@ -2901,23 +2977,23 @@
       <c r="S31">
         <v>2.48</v>
       </c>
-      <c r="T31" s="38">
+      <c r="T31" s="57">
         <v>2.65</v>
       </c>
-      <c r="U31" s="38">
+      <c r="U31" s="57">
         <f>T31/200</f>
         <v>1.325E-2</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
       </c>
       <c r="D32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -2941,10 +3017,10 @@
         <v>45</v>
       </c>
       <c r="O32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q32">
         <v>0.17</v>
@@ -2955,8 +3031,8 @@
       <c r="S32">
         <v>0.17</v>
       </c>
-      <c r="T32" s="38"/>
-      <c r="U32" s="38"/>
+      <c r="T32" s="57"/>
+      <c r="U32" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2984,7 +3060,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2997,7 +3073,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -3006,13 +3082,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -3185,7 +3261,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C10">
         <f>SUM(C2:C9)</f>
@@ -3201,7 +3277,7 @@
         <v>22</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H10" s="1">
         <f>C10*E10*F10</f>
@@ -3210,10 +3286,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>2</v>
@@ -3222,11 +3298,11 @@
         <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -3273,7 +3349,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C15">
         <v>12</v>
@@ -3294,7 +3370,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C16">
         <v>9</v>
@@ -3336,7 +3412,7 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="G18" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H18" s="1">
         <f>SUM(G13:G17)</f>
@@ -3352,8 +3428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3362,69 +3438,72 @@
     <col min="2" max="2" width="42.81640625" customWidth="1"/>
     <col min="3" max="3" width="21.08984375" customWidth="1"/>
     <col min="4" max="4" width="31.26953125" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" customWidth="1"/>
     <col min="6" max="6" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="O1" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="P1" s="1"/>
       <c r="Q1" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>85</v>
@@ -3439,7 +3518,7 @@
         <v>20.6</v>
       </c>
       <c r="H2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J2">
         <v>21.1</v>
@@ -3453,26 +3532,29 @@
       <c r="M2">
         <v>618</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2">
+        <f>(M2/1000)*P3</f>
+        <v>6.4828200000000002</v>
+      </c>
+      <c r="O2" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="O2">
+      <c r="P2" s="52">
         <v>8.92</v>
       </c>
-      <c r="P2" s="21"/>
       <c r="Q2">
         <v>0.85</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>83</v>
@@ -3487,7 +3569,7 @@
         <v>14.5</v>
       </c>
       <c r="H3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J3">
         <v>15.6</v>
@@ -3501,23 +3583,25 @@
       <c r="M3">
         <v>601</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="O3">
+      <c r="P3" s="52">
         <v>10.49</v>
       </c>
-      <c r="P3" s="21"/>
-    </row>
-    <row r="4" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="Q3">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>86</v>
@@ -3532,7 +3616,7 @@
         <v>19.600000000000001</v>
       </c>
       <c r="H4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J4">
         <v>21.05</v>
@@ -3546,23 +3630,22 @@
       <c r="M4">
         <v>615</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="O4">
+      <c r="P4" s="54">
         <v>19.3</v>
       </c>
-      <c r="P4" s="21"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>84</v>
@@ -3577,7 +3660,7 @@
         <v>14.3</v>
       </c>
       <c r="H5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J5">
         <v>16.149999999999999</v>
@@ -3597,10 +3680,10 @@
         <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>72</v>
@@ -3629,10 +3712,10 @@
         <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>73</v>
@@ -3641,22 +3724,22 @@
         <v>308.43</v>
       </c>
       <c r="F7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="H7">
         <v>29.4</v>
       </c>
       <c r="I7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="J7">
         <v>18.649999999999999</v>
       </c>
       <c r="L7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="M7">
         <v>117992</v>
@@ -3670,33 +3753,33 @@
         <v>62</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E8" s="1">
         <v>4.3899999999999997</v>
       </c>
       <c r="F8" t="s">
+        <v>258</v>
+      </c>
+      <c r="H8" t="s">
+        <v>262</v>
+      </c>
+      <c r="L8" t="s">
         <v>259</v>
-      </c>
-      <c r="H8" t="s">
-        <v>263</v>
-      </c>
-      <c r="L8" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>5</v>
@@ -3711,7 +3794,7 @@
         <v>75</v>
       </c>
       <c r="L9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
@@ -3722,7 +3805,7 @@
         <v>62</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>74</v>
@@ -3737,7 +3820,7 @@
         <v>75</v>
       </c>
       <c r="L10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
@@ -3748,7 +3831,7 @@
         <v>63</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>76</v>
@@ -3763,7 +3846,7 @@
         <v>81.5</v>
       </c>
       <c r="H11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="L11">
         <v>95763</v>
@@ -3780,7 +3863,7 @@
         <v>63</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>78</v>
@@ -3795,7 +3878,7 @@
         <v>77</v>
       </c>
       <c r="H12" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="L12">
         <v>76230</v>
@@ -3812,7 +3895,7 @@
         <v>63</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>79</v>
@@ -3827,7 +3910,7 @@
         <v>77</v>
       </c>
       <c r="H13" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="L13">
         <v>95762.5</v>
@@ -3844,7 +3927,7 @@
         <v>63</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>78</v>
@@ -3859,7 +3942,7 @@
         <v>58</v>
       </c>
       <c r="H14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L14">
         <f>185*58*2</f>
@@ -3872,28 +3955,28 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E15" s="1">
         <v>4.79</v>
       </c>
       <c r="G15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M15">
         <v>662.68</v>
@@ -3901,28 +3984,28 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E16" s="1">
         <v>1.75</v>
       </c>
       <c r="G16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M16">
         <v>158.75</v>
@@ -3930,28 +4013,28 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E17" s="1">
         <v>21.15</v>
       </c>
       <c r="G17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K17">
         <v>271.75</v>
       </c>
       <c r="L17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M17">
         <v>1920.89</v>
@@ -3959,13 +4042,13 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E18" s="1">
         <v>0.41</v>
@@ -3974,7 +4057,7 @@
         <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -3992,13 +4075,13 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E19" s="1">
         <v>1.03</v>
@@ -4007,7 +4090,7 @@
         <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -4030,7 +4113,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>68</v>
@@ -4103,7 +4186,7 @@
         <v>0.31351351351351353</v>
       </c>
       <c r="B38" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -4112,7 +4195,7 @@
         <v>0.34680851063829787</v>
       </c>
       <c r="B39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -4121,7 +4204,7 @@
         <v>0.3888888888888889</v>
       </c>
       <c r="B40" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -4130,7 +4213,7 @@
         <v>0.34973697101356677</v>
       </c>
       <c r="B41" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -4139,7 +4222,7 @@
         <v>0.34615384615384615</v>
       </c>
       <c r="B42" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>